<commit_message>
Gros commit pour je sais pas quelle raison...
</commit_message>
<xml_diff>
--- a/test_env/init_test/tdf.xlsx
+++ b/test_env/init_test/tdf.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t xml:space="preserve">       # paiement partiel facture normale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_whenGetLastTransactions_thenGetLastNTransactionsAndAnteriorBalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test – value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_whenGetTransaction_thenTransactionHaveBalance</t>
   </si>
 </sst>
 </file>
@@ -154,6 +163,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -305,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -907,12 +917,24 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G21" s="0" t="n">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="0" t="n">
         <v>1766.1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="0" t="n">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="0" t="n">
         <v>761.29</v>
       </c>
     </row>

</xml_diff>